<commit_message>
Added after-upload view and sanitized input
</commit_message>
<xml_diff>
--- a/importPresentatie.xlsx
+++ b/importPresentatie.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kaart\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="20010" windowHeight="8025"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20010" windowHeight="8025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -1450,8 +1455,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1498,7 +1503,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1506,14 +1511,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1551,9 +1559,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1585,9 +1593,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1619,9 +1628,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1794,14 +1804,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
@@ -1809,7 +1819,7 @@
     <col min="10" max="10" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1847,7 +1857,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1885,7 +1895,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1923,7 +1933,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>253</v>
       </c>
@@ -1961,7 +1971,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>254</v>
       </c>
@@ -1999,7 +2009,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>255</v>
       </c>
@@ -2037,7 +2047,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>256</v>
       </c>
@@ -2075,7 +2085,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>257</v>
       </c>
@@ -2113,7 +2123,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>259</v>
       </c>
@@ -2151,7 +2161,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>258</v>
       </c>
@@ -2189,7 +2199,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>260</v>
       </c>
@@ -2227,7 +2237,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>261</v>
       </c>
@@ -2265,7 +2275,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>262</v>
       </c>
@@ -2303,7 +2313,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>263</v>
       </c>
@@ -2341,7 +2351,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>264</v>
       </c>
@@ -2379,7 +2389,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>265</v>
       </c>
@@ -2417,7 +2427,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>266</v>
       </c>
@@ -2455,7 +2465,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>267</v>
       </c>
@@ -2493,7 +2503,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>268</v>
       </c>
@@ -2531,7 +2541,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>269</v>
       </c>
@@ -2569,7 +2579,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>270</v>
       </c>
@@ -2607,7 +2617,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>271</v>
       </c>
@@ -2645,7 +2655,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>272</v>
       </c>
@@ -2683,7 +2693,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>273</v>
       </c>
@@ -2721,7 +2731,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>274</v>
       </c>
@@ -2759,7 +2769,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>275</v>
       </c>
@@ -2797,7 +2807,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>276</v>
       </c>
@@ -2835,7 +2845,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>277</v>
       </c>
@@ -2873,7 +2883,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>278</v>
       </c>
@@ -2948,14 +2958,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90.85546875" customWidth="1"/>
@@ -2971,7 +2981,7 @@
     <col min="12" max="12" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -3009,7 +3019,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3047,7 +3057,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -3085,7 +3095,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -3123,7 +3133,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>106</v>
       </c>
@@ -3161,7 +3171,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -3199,7 +3209,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -3237,7 +3247,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>109</v>
       </c>
@@ -3275,7 +3285,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -3313,7 +3323,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>111</v>
       </c>
@@ -3351,7 +3361,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>112</v>
       </c>
@@ -3389,7 +3399,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -3427,7 +3437,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>114</v>
       </c>
@@ -3465,7 +3475,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>115</v>
       </c>
@@ -3503,7 +3513,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -3541,7 +3551,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>117</v>
       </c>
@@ -3579,7 +3589,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>118</v>
       </c>
@@ -3617,7 +3627,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -3655,7 +3665,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>120</v>
       </c>
@@ -3693,7 +3703,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -3731,7 +3741,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>122</v>
       </c>
@@ -3769,7 +3779,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>123</v>
       </c>
@@ -3807,7 +3817,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -3845,7 +3855,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>124</v>
       </c>
@@ -3883,7 +3893,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>283</v>
       </c>
@@ -3921,7 +3931,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>284</v>
       </c>
@@ -3959,7 +3969,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>285</v>
       </c>
@@ -3997,7 +4007,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>286</v>
       </c>
@@ -4035,7 +4045,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>287</v>
       </c>
@@ -4073,7 +4083,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>288</v>
       </c>
@@ -4111,7 +4121,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>289</v>
       </c>
@@ -4149,7 +4159,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>290</v>
       </c>
@@ -4187,7 +4197,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>291</v>
       </c>
@@ -4225,7 +4235,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>292</v>
       </c>
@@ -4263,7 +4273,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>293</v>
       </c>
@@ -4301,7 +4311,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>295</v>
       </c>
@@ -4339,7 +4349,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>294</v>
       </c>
@@ -4377,7 +4387,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>296</v>
       </c>
@@ -4415,7 +4425,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>297</v>
       </c>
@@ -4453,7 +4463,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>298</v>
       </c>
@@ -4491,7 +4501,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>299</v>
       </c>
@@ -4529,7 +4539,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>300</v>
       </c>
@@ -4567,7 +4577,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>301</v>
       </c>
@@ -4605,7 +4615,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>302</v>
       </c>
@@ -4643,7 +4653,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>303</v>
       </c>
@@ -4681,7 +4691,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>128</v>
       </c>
@@ -4719,7 +4729,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>304</v>
       </c>
@@ -4757,7 +4767,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>305</v>
       </c>
@@ -4795,7 +4805,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>306</v>
       </c>
@@ -4833,7 +4843,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>307</v>
       </c>
@@ -4871,7 +4881,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>308</v>
       </c>
@@ -4909,7 +4919,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>309</v>
       </c>
@@ -4947,7 +4957,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>129</v>
       </c>
@@ -4985,7 +4995,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>310</v>
       </c>
@@ -5023,7 +5033,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>311</v>
       </c>
@@ -5061,7 +5071,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>312</v>
       </c>
@@ -5099,7 +5109,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>313</v>
       </c>
@@ -5137,7 +5147,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>314</v>
       </c>
@@ -5175,7 +5185,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>315</v>
       </c>
@@ -5213,7 +5223,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>316</v>
       </c>
@@ -5251,7 +5261,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>317</v>
       </c>
@@ -5289,7 +5299,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>318</v>
       </c>
@@ -5327,7 +5337,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>319</v>
       </c>
@@ -5365,7 +5375,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J64" s="2"/>
     </row>
   </sheetData>
@@ -5439,14 +5449,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -5456,7 +5466,7 @@
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -5476,7 +5486,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -5496,7 +5506,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -5516,7 +5526,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>253</v>
       </c>
@@ -5536,7 +5546,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>254</v>
       </c>
@@ -5562,14 +5572,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
@@ -5579,7 +5589,7 @@
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -5602,9 +5612,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -5625,9 +5635,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5648,9 +5658,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -5671,9 +5681,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>127</v>
       </c>
       <c r="B5">
         <v>5</v>

</xml_diff>

<commit_message>
fixed sanitized data bug
</commit_message>
<xml_diff>
--- a/importPresentatie.xlsx
+++ b/importPresentatie.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kaart\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="20010" windowHeight="8025" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20010" windowHeight="8025"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -1561,7 +1556,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1596,7 +1591,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1807,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1900,7 +1895,7 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>132</v>
@@ -1938,7 +1933,7 @@
         <v>253</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>133</v>
@@ -1976,7 +1971,7 @@
         <v>254</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
         <v>134</v>
@@ -2204,7 +2199,7 @@
         <v>260</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>475</v>
       </c>
       <c r="C11" t="s">
         <v>135</v>
@@ -2394,7 +2389,7 @@
         <v>265</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>475</v>
       </c>
       <c r="C16" t="s">
         <v>144</v>
@@ -2432,7 +2427,7 @@
         <v>266</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>475</v>
       </c>
       <c r="C17" t="s">
         <v>145</v>
@@ -2546,7 +2541,7 @@
         <v>269</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>475</v>
       </c>
       <c r="C20" t="s">
         <v>148</v>
@@ -2660,7 +2655,7 @@
         <v>272</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>475</v>
       </c>
       <c r="C23" t="s">
         <v>151</v>
@@ -2698,7 +2693,7 @@
         <v>273</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>475</v>
       </c>
       <c r="C24" t="s">
         <v>152</v>
@@ -2961,7 +2956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>

</xml_diff>